<commit_message>
tasbhaDialog instead of tasbhaWindow, odas eltagaly, tasbha sanawy
</commit_message>
<xml_diff>
--- a/Files Data.xlsx
+++ b/Files Data.xlsx
@@ -470,7 +470,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E474"/>
+  <dimension ref="A1:E477"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4250,7 +4250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" ht="19.5" customHeight="1">
+    <row r="180" ht="18.75" customHeight="1">
       <c r="A180" t="inlineStr">
         <is>
           <t>مرد مزمور الختان</t>
@@ -4271,7 +4271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" ht="19.5" customHeight="1">
+    <row r="181" ht="18.75" customHeight="1">
       <c r="A181" t="inlineStr">
         <is>
           <t>مرد مزمور الغطاس</t>
@@ -4292,7 +4292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" ht="19.5" customHeight="1">
+    <row r="182" ht="18.75" customHeight="1">
       <c r="A182" t="inlineStr">
         <is>
           <t>مرد مزمور عرس قانا الجليل</t>
@@ -4313,7 +4313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" ht="19.5" customHeight="1">
+    <row r="183" ht="18.75" customHeight="1">
       <c r="A183" t="inlineStr">
         <is>
           <t>مرد مزمور دخول المسيح الهيكل</t>
@@ -4334,7 +4334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" ht="19.5" customHeight="1">
+    <row r="184" ht="18.75" customHeight="1">
       <c r="A184" t="inlineStr">
         <is>
           <t>مرد مزمور البشارة</t>
@@ -4355,7 +4355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" ht="19.5" customHeight="1">
+    <row r="185" ht="18.75" customHeight="1">
       <c r="A185" t="inlineStr">
         <is>
           <t>مرد مزمور الشعانين</t>
@@ -4376,7 +4376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" ht="19.5" customHeight="1">
+    <row r="186" ht="18.75" customHeight="1">
       <c r="A186" t="inlineStr">
         <is>
           <t>مرد المزمور القيامة</t>
@@ -4397,7 +4397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" ht="19.5" customHeight="1">
+    <row r="187" ht="18.75" customHeight="1">
       <c r="A187" t="inlineStr">
         <is>
           <t>مرد مزمور الصعود</t>
@@ -4418,7 +4418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" ht="19.5" customHeight="1">
+    <row r="188" ht="18.75" customHeight="1">
       <c r="A188" t="inlineStr">
         <is>
           <t>مرد مزمور العنصرة</t>
@@ -9314,187 +9314,187 @@
     <row r="421" ht="18.75" customHeight="1">
       <c r="A421" t="inlineStr">
         <is>
-          <t>قسمة أعياد الملائكة والسيدة العذراء وسنوى (هوذا كائن معنا على هذه)</t>
+          <t>قسمة للإبن تُقال في عيد التجلي (أنت هو كلمة الآب)</t>
         </is>
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>{71232865-63AA-40C5-8F02-BABBFE7297D3}</t>
+          <t>{C23F094B-BD4E-4348-8186-D1C4B8744FAA}</t>
         </is>
       </c>
       <c r="C421" t="n">
         <v>3082</v>
       </c>
       <c r="D421" t="n">
-        <v>3090</v>
+        <v>3087</v>
       </c>
       <c r="E421" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="422" ht="18.75" customHeight="1">
       <c r="A422" t="inlineStr">
         <is>
-          <t>صوم و أعياد القديسة العذراء مريم (يا الله الساكن في الأعالي)</t>
+          <t>قسمة أعياد الملائكة والسيدة العذراء وسنوى (هوذا كائن معنا على هذه)</t>
         </is>
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>{C78EDE33-ED5C-411D-A2E6-2B55E70B9F6B}</t>
+          <t>{71232865-63AA-40C5-8F02-BABBFE7297D3}</t>
         </is>
       </c>
       <c r="C422" t="n">
-        <v>3091</v>
+        <v>3088</v>
       </c>
       <c r="D422" t="n">
-        <v>3104</v>
+        <v>3096</v>
       </c>
       <c r="E422" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="423" ht="18.75" customHeight="1">
       <c r="A423" t="inlineStr">
         <is>
-          <t>قسمة للإبن تقال في الأعياد السيدية وسنوى (نسبح ونمجد إله الآلهة)</t>
+          <t>صوم و أعياد القديسة العذراء مريم (يا الله الساكن في الأعالي)</t>
         </is>
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>{2A09ADD1-849A-4776-9FF5-9E0F56C9BAED}</t>
+          <t>{C78EDE33-ED5C-411D-A2E6-2B55E70B9F6B}</t>
         </is>
       </c>
       <c r="C423" t="n">
-        <v>3105</v>
+        <v>3097</v>
       </c>
       <c r="D423" t="n">
-        <v>3112</v>
+        <v>3110</v>
       </c>
       <c r="E423" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="424" ht="18.75" customHeight="1">
       <c r="A424" t="inlineStr">
         <is>
-          <t>قسمة تذكار البشارة والميلاد والقيامة (نسبح ونمجد إله الآلهة ورب الأرباب)</t>
+          <t>قسمة للإبن تقال في الأعياد السيدية وسنوى (نسبح ونمجد إله الآلهة)</t>
         </is>
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>{BCFF601E-ED54-486A-9884-027CD11CA3C0}</t>
+          <t>{2A09ADD1-849A-4776-9FF5-9E0F56C9BAED}</t>
         </is>
       </c>
       <c r="C424" t="n">
-        <v>3113</v>
+        <v>3111</v>
       </c>
       <c r="D424" t="n">
-        <v>3122</v>
+        <v>3118</v>
       </c>
       <c r="E424" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="425" ht="18.75" customHeight="1">
       <c r="A425" t="inlineStr">
         <is>
-          <t>ابانا الذي في السموات</t>
+          <t>قسمة تذكار البشارة والميلاد والقيامة (نسبح ونمجد إله الآلهة ورب الأرباب)</t>
         </is>
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>{F8657D52-0E61-475D-90AC-DB10509A5D22}</t>
+          <t>{BCFF601E-ED54-486A-9884-027CD11CA3C0}</t>
         </is>
       </c>
       <c r="C425" t="n">
-        <v>3123</v>
+        <v>3119</v>
       </c>
       <c r="D425" t="n">
         <v>3128</v>
       </c>
       <c r="E425" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="426" ht="18.75" customHeight="1">
       <c r="A426" t="inlineStr">
         <is>
-          <t>ما قبل الإعتراف</t>
+          <t>ابانا الذي في السموات</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>{80F60976-3BEB-4133-A7EB-026E12D4799C}</t>
+          <t>{F8657D52-0E61-475D-90AC-DB10509A5D22}</t>
         </is>
       </c>
       <c r="C426" t="n">
         <v>3129</v>
       </c>
       <c r="D426" t="n">
-        <v>3153</v>
+        <v>3134</v>
       </c>
       <c r="E426" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="427" ht="18.75" customHeight="1">
       <c r="A427" t="inlineStr">
         <is>
-          <t>الاعتراف</t>
+          <t>ما قبل الإعتراف</t>
         </is>
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>{EE8004CA-FF9E-4471-963C-7F0946AE78FC}</t>
+          <t>{80F60976-3BEB-4133-A7EB-026E12D4799C}</t>
         </is>
       </c>
       <c r="C427" t="n">
-        <v>3154</v>
+        <v>3135</v>
       </c>
       <c r="D427" t="n">
-        <v>3177</v>
+        <v>3159</v>
       </c>
       <c r="E427" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="428" ht="18.75" customHeight="1">
       <c r="A428" t="inlineStr">
         <is>
-          <t>مرد توزيع النيروز</t>
+          <t>الاعتراف</t>
         </is>
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>{76AC6D29-E354-4FF7-AA9F-EA0B71399749}</t>
+          <t>{EE8004CA-FF9E-4471-963C-7F0946AE78FC}</t>
         </is>
       </c>
       <c r="C428" t="n">
-        <v>3178</v>
+        <v>3160</v>
       </c>
       <c r="D428" t="n">
-        <v>3178</v>
+        <v>3183</v>
       </c>
       <c r="E428" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="429" ht="18.75" customHeight="1">
       <c r="A429" t="inlineStr">
         <is>
-          <t>مرد توزيع الصليب</t>
+          <t>مرد توزيع النيروز</t>
         </is>
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>{E4E79CE2-AD28-44FB-B8B3-6B59A5D64B62}</t>
+          <t>{76AC6D29-E354-4FF7-AA9F-EA0B71399749}</t>
         </is>
       </c>
       <c r="C429" t="n">
-        <v>3179</v>
+        <v>3184</v>
       </c>
       <c r="D429" t="n">
-        <v>3179</v>
+        <v>3184</v>
       </c>
       <c r="E429" t="n">
         <v>1</v>
@@ -9503,19 +9503,19 @@
     <row r="430" ht="18.75" customHeight="1">
       <c r="A430" t="inlineStr">
         <is>
-          <t>مرد توزيع الغطاس</t>
+          <t>مرد توزيع الصليب</t>
         </is>
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>{96A65364-75BE-44B2-A2D8-29785DBD26C4}</t>
+          <t>{E4E79CE2-AD28-44FB-B8B3-6B59A5D64B62}</t>
         </is>
       </c>
       <c r="C430" t="n">
-        <v>3180</v>
+        <v>3185</v>
       </c>
       <c r="D430" t="n">
-        <v>3180</v>
+        <v>3185</v>
       </c>
       <c r="E430" t="n">
         <v>1</v>
@@ -9524,19 +9524,19 @@
     <row r="431" ht="18.75" customHeight="1">
       <c r="A431" t="inlineStr">
         <is>
-          <t>مرد توزيع الختان</t>
+          <t>مرد توزيع الغطاس</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>{3ED0ED6F-B67A-410E-958B-1437069EE8B5}</t>
+          <t>{96A65364-75BE-44B2-A2D8-29785DBD26C4}</t>
         </is>
       </c>
       <c r="C431" t="n">
-        <v>3181</v>
+        <v>3186</v>
       </c>
       <c r="D431" t="n">
-        <v>3181</v>
+        <v>3186</v>
       </c>
       <c r="E431" t="n">
         <v>1</v>
@@ -9545,19 +9545,19 @@
     <row r="432" ht="18.75" customHeight="1">
       <c r="A432" t="inlineStr">
         <is>
-          <t>مرد توزيع عرس قانا الجليل</t>
+          <t>مرد توزيع الختان</t>
         </is>
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>{DACB52D6-560B-4038-BDA3-7A7315DEA6D0}</t>
+          <t>{3ED0ED6F-B67A-410E-958B-1437069EE8B5}</t>
         </is>
       </c>
       <c r="C432" t="n">
-        <v>3182</v>
+        <v>3187</v>
       </c>
       <c r="D432" t="n">
-        <v>3182</v>
+        <v>3187</v>
       </c>
       <c r="E432" t="n">
         <v>1</v>
@@ -9566,19 +9566,19 @@
     <row r="433" ht="18.75" customHeight="1">
       <c r="A433" t="inlineStr">
         <is>
-          <t>مرد توزيع دخول المسيح الهيكل</t>
+          <t>مرد توزيع عرس قانا الجليل</t>
         </is>
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>{49900A3A-E6E6-4152-84C8-B741F3C50853}</t>
+          <t>{DACB52D6-560B-4038-BDA3-7A7315DEA6D0}</t>
         </is>
       </c>
       <c r="C433" t="n">
-        <v>3183</v>
+        <v>3188</v>
       </c>
       <c r="D433" t="n">
-        <v>3183</v>
+        <v>3188</v>
       </c>
       <c r="E433" t="n">
         <v>1</v>
@@ -9587,19 +9587,19 @@
     <row r="434" ht="18.75" customHeight="1">
       <c r="A434" t="inlineStr">
         <is>
-          <t>مرد توزيع صوم نينوى</t>
+          <t>مرد توزيع دخول المسيح الهيكل</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>{8B7ED515-48EF-40B6-B9F2-80B8A4CC1126}</t>
+          <t>{49900A3A-E6E6-4152-84C8-B741F3C50853}</t>
         </is>
       </c>
       <c r="C434" t="n">
-        <v>3184</v>
+        <v>3189</v>
       </c>
       <c r="D434" t="n">
-        <v>3184</v>
+        <v>3189</v>
       </c>
       <c r="E434" t="n">
         <v>1</v>
@@ -9608,19 +9608,19 @@
     <row r="435" ht="18.75" customHeight="1">
       <c r="A435" t="inlineStr">
         <is>
-          <t>مرد توزيع الصوم الكبير</t>
+          <t>مرد توزيع صوم نينوى</t>
         </is>
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>{F9ED982E-F6FB-4E2B-8955-C5E80C70C2D6}</t>
+          <t>{8B7ED515-48EF-40B6-B9F2-80B8A4CC1126}</t>
         </is>
       </c>
       <c r="C435" t="n">
-        <v>3185</v>
+        <v>3190</v>
       </c>
       <c r="D435" t="n">
-        <v>3185</v>
+        <v>3190</v>
       </c>
       <c r="E435" t="n">
         <v>1</v>
@@ -9629,19 +9629,19 @@
     <row r="436" ht="18.75" customHeight="1">
       <c r="A436" t="inlineStr">
         <is>
-          <t>مرد توزيع الشعانين</t>
+          <t>مرد توزيع الصوم الكبير</t>
         </is>
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>{C95D30EC-C174-40B5-8671-08FA653E3199}</t>
+          <t>{F9ED982E-F6FB-4E2B-8955-C5E80C70C2D6}</t>
         </is>
       </c>
       <c r="C436" t="n">
-        <v>3186</v>
+        <v>3191</v>
       </c>
       <c r="D436" t="n">
-        <v>3186</v>
+        <v>3191</v>
       </c>
       <c r="E436" t="n">
         <v>1</v>
@@ -9650,19 +9650,19 @@
     <row r="437" ht="18.75" customHeight="1">
       <c r="A437" t="inlineStr">
         <is>
-          <t>مرد توزيع البشارة</t>
+          <t>مرد توزيع الشعانين</t>
         </is>
       </c>
       <c r="B437" t="inlineStr">
         <is>
-          <t>{2F035E60-4CC5-4808-A906-367BDB0FC9B0}</t>
+          <t>{C95D30EC-C174-40B5-8671-08FA653E3199}</t>
         </is>
       </c>
       <c r="C437" t="n">
-        <v>3187</v>
+        <v>3192</v>
       </c>
       <c r="D437" t="n">
-        <v>3187</v>
+        <v>3192</v>
       </c>
       <c r="E437" t="n">
         <v>1</v>
@@ -9671,19 +9671,19 @@
     <row r="438" ht="18.75" customHeight="1">
       <c r="A438" t="inlineStr">
         <is>
-          <t>مرد توزيع الميلاد</t>
+          <t>مرد توزيع البشارة</t>
         </is>
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>{D10973F3-B5C6-431E-8EDA-60ABA7A98C9E}</t>
+          <t>{2F035E60-4CC5-4808-A906-367BDB0FC9B0}</t>
         </is>
       </c>
       <c r="C438" t="n">
-        <v>3188</v>
+        <v>3193</v>
       </c>
       <c r="D438" t="n">
-        <v>3188</v>
+        <v>3193</v>
       </c>
       <c r="E438" t="n">
         <v>1</v>
@@ -9692,19 +9692,19 @@
     <row r="439" ht="18.75" customHeight="1">
       <c r="A439" t="inlineStr">
         <is>
-          <t>مرد توزيع القيامة</t>
+          <t>مرد توزيع الميلاد</t>
         </is>
       </c>
       <c r="B439" t="inlineStr">
         <is>
-          <t>{AB0FAC0A-1DAB-4ABD-BAA1-7557AA4860AA}</t>
+          <t>{D10973F3-B5C6-431E-8EDA-60ABA7A98C9E}</t>
         </is>
       </c>
       <c r="C439" t="n">
-        <v>3189</v>
+        <v>3194</v>
       </c>
       <c r="D439" t="n">
-        <v>3189</v>
+        <v>3194</v>
       </c>
       <c r="E439" t="n">
         <v>1</v>
@@ -9713,19 +9713,19 @@
     <row r="440" ht="18.75" customHeight="1">
       <c r="A440" t="inlineStr">
         <is>
-          <t>مرد توزيع الصعود</t>
+          <t>مرد توزيع القيامة</t>
         </is>
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>{834F8F17-CEC0-4E51-A927-8074D22B6A78}</t>
+          <t>{AB0FAC0A-1DAB-4ABD-BAA1-7557AA4860AA}</t>
         </is>
       </c>
       <c r="C440" t="n">
-        <v>3190</v>
+        <v>3195</v>
       </c>
       <c r="D440" t="n">
-        <v>3190</v>
+        <v>3195</v>
       </c>
       <c r="E440" t="n">
         <v>1</v>
@@ -9734,19 +9734,19 @@
     <row r="441" ht="18.75" customHeight="1">
       <c r="A441" t="inlineStr">
         <is>
-          <t>مرد توزيع العنصرة</t>
+          <t>مرد توزيع الصعود</t>
         </is>
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>{22674B27-BBD5-49D8-98B9-ABCA6F4C5504}</t>
+          <t>{834F8F17-CEC0-4E51-A927-8074D22B6A78}</t>
         </is>
       </c>
       <c r="C441" t="n">
-        <v>3191</v>
+        <v>3196</v>
       </c>
       <c r="D441" t="n">
-        <v>3191</v>
+        <v>3196</v>
       </c>
       <c r="E441" t="n">
         <v>1</v>
@@ -9755,166 +9755,166 @@
     <row r="442" ht="18.75" customHeight="1">
       <c r="A442" t="inlineStr">
         <is>
-          <t>مزمور التوزيع</t>
+          <t>مرد توزيع العنصرة</t>
         </is>
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>{C29E5A83-A98B-4077-8194-99A6D803EF53}</t>
+          <t>{22674B27-BBD5-49D8-98B9-ABCA6F4C5504}</t>
         </is>
       </c>
       <c r="C442" t="n">
-        <v>3192</v>
+        <v>3197</v>
       </c>
       <c r="D442" t="n">
-        <v>3208</v>
+        <v>3197</v>
       </c>
       <c r="E442" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="443" ht="18.75" customHeight="1">
       <c r="A443" t="inlineStr">
         <is>
-          <t>اطاي بارثينوس</t>
+          <t>مرد توزيع التجلي</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>{18835C90-087E-4BAC-9D66-708BC1E04983}</t>
+          <t>{0080F7D2-9802-4100-8B27-DD23FBF42BCF}</t>
         </is>
       </c>
       <c r="C443" t="n">
-        <v>3209</v>
+        <v>3198</v>
       </c>
       <c r="D443" t="n">
-        <v>3230</v>
+        <v>3198</v>
       </c>
       <c r="E443" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="444" ht="18.75" customHeight="1">
       <c r="A444" t="inlineStr">
         <is>
-          <t>لازاروس</t>
+          <t>مزمور التوزيع</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>{78C64C43-B3F6-4110-8CB0-1E10086C77C2}</t>
+          <t>{C29E5A83-A98B-4077-8194-99A6D803EF53}</t>
         </is>
       </c>
       <c r="C444" t="n">
-        <v>3231</v>
+        <v>3199</v>
       </c>
       <c r="D444" t="n">
-        <v>3258</v>
+        <v>3215</v>
       </c>
       <c r="E444" t="n">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="445" ht="18.75" customHeight="1">
       <c r="A445" t="inlineStr">
         <is>
-          <t>كاطا ني خوروس</t>
+          <t>اطاي بارثينوس</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>{8E020F97-3459-40AC-828C-13346E2C46B1}</t>
+          <t>{18835C90-087E-4BAC-9D66-708BC1E04983}</t>
         </is>
       </c>
       <c r="C445" t="n">
-        <v>3259</v>
+        <v>3216</v>
       </c>
       <c r="D445" t="n">
-        <v>3262</v>
+        <v>3237</v>
       </c>
       <c r="E445" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="446" ht="18.75" customHeight="1">
       <c r="A446" t="inlineStr">
         <is>
-          <t>فهرس الحان التوزيع</t>
+          <t>لازاروس</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>{688FAD52-7F6A-4FA9-8CF7-EBB80B3B6069}</t>
+          <t>{78C64C43-B3F6-4110-8CB0-1E10086C77C2}</t>
         </is>
       </c>
       <c r="C446" t="n">
-        <v>3263</v>
+        <v>3238</v>
       </c>
       <c r="D446" t="n">
-        <v>3263</v>
+        <v>3265</v>
       </c>
       <c r="E446" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="447" ht="18.75" customHeight="1">
       <c r="A447" t="inlineStr">
         <is>
-          <t>اك اسماروؤت</t>
+          <t>كاطا ني خوروس</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t>{507EFD97-98F8-4376-848B-20D72E16D2C1}</t>
+          <t>{8E020F97-3459-40AC-828C-13346E2C46B1}</t>
         </is>
       </c>
       <c r="C447" t="n">
-        <v>3264</v>
+        <v>3266</v>
       </c>
       <c r="D447" t="n">
-        <v>3265</v>
+        <v>3269</v>
       </c>
       <c r="E447" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="448" ht="18.75" customHeight="1">
       <c r="A448" t="inlineStr">
         <is>
-          <t>بي اويك</t>
+          <t>فهرس الحان التوزيع</t>
         </is>
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t>{B9A30F5E-0C89-471B-A99A-23DBE7F58504}</t>
+          <t>{688FAD52-7F6A-4FA9-8CF7-EBB80B3B6069}</t>
         </is>
       </c>
       <c r="C448" t="n">
-        <v>3266</v>
+        <v>3270</v>
       </c>
       <c r="D448" t="n">
-        <v>3276</v>
+        <v>3270</v>
       </c>
       <c r="E448" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="449" ht="18.75" customHeight="1">
       <c r="A449" t="inlineStr">
         <is>
-          <t>جي اف اسماروؤت</t>
+          <t>اك اسماروؤت</t>
         </is>
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t>{82450F2E-38A9-42FB-ACFD-B874384545D2}</t>
+          <t>{507EFD97-98F8-4376-848B-20D72E16D2C1}</t>
         </is>
       </c>
       <c r="C449" t="n">
-        <v>3277</v>
+        <v>3271</v>
       </c>
       <c r="D449" t="n">
-        <v>3278</v>
+        <v>3272</v>
       </c>
       <c r="E449" t="n">
         <v>2</v>
@@ -9923,187 +9923,187 @@
     <row r="450" ht="18.75" customHeight="1">
       <c r="A450" t="inlineStr">
         <is>
-          <t>اسومين</t>
+          <t>بي اويك</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
         <is>
-          <t>{3F22DD0B-D926-42B9-BABE-6C6486C9BD62}</t>
+          <t>{B9A30F5E-0C89-471B-A99A-23DBE7F58504}</t>
         </is>
       </c>
       <c r="C450" t="n">
-        <v>3279</v>
+        <v>3273</v>
       </c>
       <c r="D450" t="n">
-        <v>3303</v>
+        <v>3283</v>
       </c>
       <c r="E450" t="n">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="451" ht="18.75" customHeight="1">
       <c r="A451" t="inlineStr">
         <is>
-          <t>اف امبشا غار</t>
+          <t>جي اف اسماروؤت</t>
         </is>
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>{87BCA258-F572-4FEC-97DE-71CBA3159BB9}</t>
+          <t>{82450F2E-38A9-42FB-ACFD-B874384545D2}</t>
         </is>
       </c>
       <c r="C451" t="n">
-        <v>3304</v>
+        <v>3284</v>
       </c>
       <c r="D451" t="n">
-        <v>3342</v>
+        <v>3285</v>
       </c>
       <c r="E451" t="n">
-        <v>39</v>
+        <v>2</v>
       </c>
     </row>
     <row r="452" ht="18.75" customHeight="1">
       <c r="A452" t="inlineStr">
         <is>
-          <t>تي بارثينوس</t>
+          <t>اسومين</t>
         </is>
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>{185E1789-C295-487F-8018-CC029600A8F6}</t>
+          <t>{3F22DD0B-D926-42B9-BABE-6C6486C9BD62}</t>
         </is>
       </c>
       <c r="C452" t="n">
-        <v>3343</v>
+        <v>3286</v>
       </c>
       <c r="D452" t="n">
-        <v>3355</v>
+        <v>3310</v>
       </c>
       <c r="E452" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="453" ht="18.75" customHeight="1">
       <c r="A453" t="inlineStr">
         <is>
-          <t>يونا بى ابروفيتيس</t>
+          <t>اف امبشا غار</t>
         </is>
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>{859D33B0-D7E3-4EDC-8AB9-E56533A2D980}</t>
+          <t>{87BCA258-F572-4FEC-97DE-71CBA3159BB9}</t>
         </is>
       </c>
       <c r="C453" t="n">
-        <v>3356</v>
+        <v>3311</v>
       </c>
       <c r="D453" t="n">
-        <v>3371</v>
+        <v>3349</v>
       </c>
       <c r="E453" t="n">
-        <v>16</v>
+        <v>39</v>
       </c>
     </row>
     <row r="454" ht="18.75" customHeight="1">
       <c r="A454" t="inlineStr">
         <is>
-          <t>بي ماي رومي</t>
+          <t>تي بارثينوس</t>
         </is>
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>{315091E2-E367-43B7-A35E-4175DF947038}</t>
+          <t>{185E1789-C295-487F-8018-CC029600A8F6}</t>
         </is>
       </c>
       <c r="C454" t="n">
-        <v>3372</v>
+        <v>3350</v>
       </c>
       <c r="D454" t="n">
-        <v>3386</v>
+        <v>3362</v>
       </c>
       <c r="E454" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="455" ht="18.75" customHeight="1">
       <c r="A455" t="inlineStr">
         <is>
-          <t>اونيشتي اميستيريون</t>
+          <t>يونا بى ابروفيتيس</t>
         </is>
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>{DB680029-4B05-4C3F-98B3-FB5469AADBD7}</t>
+          <t>{859D33B0-D7E3-4EDC-8AB9-E56533A2D980}</t>
         </is>
       </c>
       <c r="C455" t="n">
-        <v>3387</v>
+        <v>3363</v>
       </c>
       <c r="D455" t="n">
-        <v>3406</v>
+        <v>3378</v>
       </c>
       <c r="E455" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="456" ht="18.75" customHeight="1">
       <c r="A456" t="inlineStr">
         <is>
-          <t>مدائح سنوي</t>
+          <t>بي ماي رومي</t>
         </is>
       </c>
       <c r="B456" t="inlineStr">
         <is>
-          <t>{07298C47-E831-4285-ACB7-25BB3772C6A2}</t>
+          <t>{315091E2-E367-43B7-A35E-4175DF947038}</t>
         </is>
       </c>
       <c r="C456" t="n">
-        <v>3407</v>
+        <v>3379</v>
       </c>
       <c r="D456" t="n">
-        <v>3407</v>
+        <v>3393</v>
       </c>
       <c r="E456" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="457" ht="18.75" customHeight="1">
       <c r="A457" t="inlineStr">
         <is>
-          <t>مدائح كيهك</t>
+          <t>اونيشتي اميستيريون</t>
         </is>
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>{DCEAD1F4-0405-4EE6-9905-219FC8E85798}</t>
+          <t>{DB680029-4B05-4C3F-98B3-FB5469AADBD7}</t>
         </is>
       </c>
       <c r="C457" t="n">
-        <v>3408</v>
+        <v>3394</v>
       </c>
       <c r="D457" t="n">
-        <v>3408</v>
+        <v>3413</v>
       </c>
       <c r="E457" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="458" ht="18.75" customHeight="1">
       <c r="A458" t="inlineStr">
         <is>
-          <t>مدائح الميلاد</t>
+          <t>مدائح سنوي</t>
         </is>
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>{42181297-997B-4C4C-B43B-4E9D8A23858D}</t>
+          <t>{07298C47-E831-4285-ACB7-25BB3772C6A2}</t>
         </is>
       </c>
       <c r="C458" t="n">
-        <v>3409</v>
+        <v>3414</v>
       </c>
       <c r="D458" t="n">
-        <v>3409</v>
+        <v>3414</v>
       </c>
       <c r="E458" t="n">
         <v>1</v>
@@ -10112,19 +10112,19 @@
     <row r="459" ht="18.75" customHeight="1">
       <c r="A459" t="inlineStr">
         <is>
-          <t>مدائح صوم نينوى</t>
+          <t>مدائح كيهك</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>{43C9AE43-EC80-4A72-97F0-F38A712DDA09}</t>
+          <t>{DCEAD1F4-0405-4EE6-9905-219FC8E85798}</t>
         </is>
       </c>
       <c r="C459" t="n">
-        <v>3410</v>
+        <v>3415</v>
       </c>
       <c r="D459" t="n">
-        <v>3410</v>
+        <v>3415</v>
       </c>
       <c r="E459" t="n">
         <v>1</v>
@@ -10133,19 +10133,19 @@
     <row r="460" ht="18.75" customHeight="1">
       <c r="A460" t="inlineStr">
         <is>
-          <t>مدائح الصوم الكبير</t>
+          <t>مدائح الميلاد</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>{6C210ECD-CC91-4984-B251-46939B2A0039}</t>
+          <t>{42181297-997B-4C4C-B43B-4E9D8A23858D}</t>
         </is>
       </c>
       <c r="C460" t="n">
-        <v>3411</v>
+        <v>3416</v>
       </c>
       <c r="D460" t="n">
-        <v>3411</v>
+        <v>3416</v>
       </c>
       <c r="E460" t="n">
         <v>1</v>
@@ -10154,19 +10154,19 @@
     <row r="461" ht="18.75" customHeight="1">
       <c r="A461" t="inlineStr">
         <is>
-          <t>مدائح سبت لعازر</t>
+          <t>مدائح صوم نينوى</t>
         </is>
       </c>
       <c r="B461" t="inlineStr">
         <is>
-          <t>{DB6B4ECA-F770-40E7-A7BA-46A8B5B46C3B}</t>
+          <t>{43C9AE43-EC80-4A72-97F0-F38A712DDA09}</t>
         </is>
       </c>
       <c r="C461" t="n">
-        <v>3412</v>
+        <v>3417</v>
       </c>
       <c r="D461" t="n">
-        <v>3412</v>
+        <v>3417</v>
       </c>
       <c r="E461" t="n">
         <v>1</v>
@@ -10175,19 +10175,19 @@
     <row r="462" ht="18.75" customHeight="1">
       <c r="A462" t="inlineStr">
         <is>
-          <t>مدائح احد الشعانين</t>
+          <t>مدائح الصوم الكبير</t>
         </is>
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>{37DC4920-98DA-477A-A6F7-6D252B149A22}</t>
+          <t>{6C210ECD-CC91-4984-B251-46939B2A0039}</t>
         </is>
       </c>
       <c r="C462" t="n">
-        <v>3413</v>
+        <v>3418</v>
       </c>
       <c r="D462" t="n">
-        <v>3413</v>
+        <v>3418</v>
       </c>
       <c r="E462" t="n">
         <v>1</v>
@@ -10196,19 +10196,19 @@
     <row r="463" ht="18.75" customHeight="1">
       <c r="A463" t="inlineStr">
         <is>
-          <t>مدائح القيامة</t>
+          <t>مدائح سبت لعازر</t>
         </is>
       </c>
       <c r="B463" t="inlineStr">
         <is>
-          <t>{1D781881-AD2E-41FE-97D4-458A86F892F1}</t>
+          <t>{DB6B4ECA-F770-40E7-A7BA-46A8B5B46C3B}</t>
         </is>
       </c>
       <c r="C463" t="n">
-        <v>3414</v>
+        <v>3419</v>
       </c>
       <c r="D463" t="n">
-        <v>3414</v>
+        <v>3419</v>
       </c>
       <c r="E463" t="n">
         <v>1</v>
@@ -10217,19 +10217,19 @@
     <row r="464" ht="18.75" customHeight="1">
       <c r="A464" t="inlineStr">
         <is>
-          <t>مدائح الخماسين من 2 الى 39</t>
+          <t>مدائح احد الشعانين</t>
         </is>
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>{F74608AC-8E8B-460A-97E7-1E6B86D50B5B}</t>
+          <t>{37DC4920-98DA-477A-A6F7-6D252B149A22}</t>
         </is>
       </c>
       <c r="C464" t="n">
-        <v>3415</v>
+        <v>3420</v>
       </c>
       <c r="D464" t="n">
-        <v>3415</v>
+        <v>3420</v>
       </c>
       <c r="E464" t="n">
         <v>1</v>
@@ -10238,19 +10238,19 @@
     <row r="465" ht="18.75" customHeight="1">
       <c r="A465" t="inlineStr">
         <is>
-          <t>مدائح الصعود الى العنصرة</t>
+          <t>مدائح القيامة</t>
         </is>
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>{BAAC56F0-C9A0-4321-AB43-D79F5FCE37C9}</t>
+          <t>{1D781881-AD2E-41FE-97D4-458A86F892F1}</t>
         </is>
       </c>
       <c r="C465" t="n">
-        <v>3416</v>
+        <v>3421</v>
       </c>
       <c r="D465" t="n">
-        <v>3416</v>
+        <v>3421</v>
       </c>
       <c r="E465" t="n">
         <v>1</v>
@@ -10259,19 +10259,19 @@
     <row r="466" ht="18.75" customHeight="1">
       <c r="A466" t="inlineStr">
         <is>
-          <t>مدائح صوم الرسل</t>
+          <t>مدائح الخماسين من 2 الى 39</t>
         </is>
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>{5F05D018-CCA5-41B9-A869-A1F64A0C2BCC}</t>
+          <t>{F74608AC-8E8B-460A-97E7-1E6B86D50B5B}</t>
         </is>
       </c>
       <c r="C466" t="n">
-        <v>3417</v>
+        <v>3422</v>
       </c>
       <c r="D466" t="n">
-        <v>3417</v>
+        <v>3422</v>
       </c>
       <c r="E466" t="n">
         <v>1</v>
@@ -10280,19 +10280,19 @@
     <row r="467" ht="18.75" customHeight="1">
       <c r="A467" t="inlineStr">
         <is>
-          <t>مدائح ال29 من الشهر</t>
+          <t>مدائح الصعود الى العنصرة</t>
         </is>
       </c>
       <c r="B467" t="inlineStr">
         <is>
-          <t>{3BE1A381-B11E-4562-921A-ECB2221D0A43}</t>
+          <t>{BAAC56F0-C9A0-4321-AB43-D79F5FCE37C9}</t>
         </is>
       </c>
       <c r="C467" t="n">
-        <v>3418</v>
+        <v>3423</v>
       </c>
       <c r="D467" t="n">
-        <v>3418</v>
+        <v>3423</v>
       </c>
       <c r="E467" t="n">
         <v>1</v>
@@ -10301,40 +10301,40 @@
     <row r="468" ht="18.75" customHeight="1">
       <c r="A468" t="inlineStr">
         <is>
-          <t>ابؤرو للتوزيع</t>
+          <t>مدائح صوم الرسل</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>{7007E16E-5DD0-4268-A326-25AF88EA4DE9}</t>
+          <t>{5F05D018-CCA5-41B9-A869-A1F64A0C2BCC}</t>
         </is>
       </c>
       <c r="C468" t="n">
-        <v>3419</v>
+        <v>3424</v>
       </c>
       <c r="D468" t="n">
-        <v>3429</v>
+        <v>3424</v>
       </c>
       <c r="E468" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="469" ht="18.75" customHeight="1">
       <c r="A469" t="inlineStr">
         <is>
-          <t>الختام</t>
+          <t>مدائح الاعياد السيدية</t>
         </is>
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>{90F50AB7-3911-445D-9C45-41866ECCCED0}</t>
+          <t>{147FD013-1F73-40AC-92A0-5544B48FA888}</t>
         </is>
       </c>
       <c r="C469" t="n">
-        <v>3430</v>
+        <v>3425</v>
       </c>
       <c r="D469" t="n">
-        <v>3430</v>
+        <v>3425</v>
       </c>
       <c r="E469" t="n">
         <v>1</v>
@@ -10343,105 +10343,168 @@
     <row r="470" ht="18.75" customHeight="1">
       <c r="A470" t="inlineStr">
         <is>
-          <t>الختام السنوي</t>
+          <t>مدائح ال29 من الشهر</t>
         </is>
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>{0D2A50D9-F484-4E60-922B-66FF81444E2C}</t>
+          <t>{3BE1A381-B11E-4562-921A-ECB2221D0A43}</t>
         </is>
       </c>
       <c r="C470" t="n">
-        <v>3431</v>
+        <v>3426</v>
       </c>
       <c r="D470" t="n">
-        <v>3433</v>
+        <v>3426</v>
       </c>
       <c r="E470" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="471" ht="18.75" customHeight="1">
       <c r="A471" t="inlineStr">
         <is>
-          <t>الختام في الصوم المقدس</t>
+          <t>ابؤرو للتوزيع</t>
         </is>
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>{4A3AE26D-6D71-4143-8C05-7618E08EF248}</t>
+          <t>{7007E16E-5DD0-4268-A326-25AF88EA4DE9}</t>
         </is>
       </c>
       <c r="C471" t="n">
-        <v>3434</v>
+        <v>3427</v>
       </c>
       <c r="D471" t="n">
-        <v>3439</v>
+        <v>3437</v>
       </c>
       <c r="E471" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="472" ht="18.75" customHeight="1">
       <c r="A472" t="inlineStr">
         <is>
-          <t>تكملة على حسب المناسبة</t>
+          <t>الختام</t>
         </is>
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>{A18EDC94-F257-4FAC-99C7-0A8EA70F0FAF}</t>
+          <t>{90F50AB7-3911-445D-9C45-41866ECCCED0}</t>
         </is>
       </c>
       <c r="C472" t="n">
-        <v>3440</v>
+        <v>3438</v>
       </c>
       <c r="D472" t="n">
-        <v>3464</v>
+        <v>3438</v>
       </c>
       <c r="E472" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="473" ht="18.75" customHeight="1">
       <c r="A473" t="inlineStr">
         <is>
-          <t>في حضور الاسقف</t>
+          <t>الختام السنوي</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>{A9183893-7B7E-459F-8547-F7A8F7D2D521}</t>
+          <t>{0D2A50D9-F484-4E60-922B-66FF81444E2C}</t>
         </is>
       </c>
       <c r="C473" t="n">
-        <v>3465</v>
+        <v>3439</v>
       </c>
       <c r="D473" t="n">
-        <v>3473</v>
+        <v>3441</v>
       </c>
       <c r="E473" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="474" ht="18.75" customHeight="1">
       <c r="A474" t="inlineStr">
         <is>
+          <t>الختام في الصوم المقدس</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>{4A3AE26D-6D71-4143-8C05-7618E08EF248}</t>
+        </is>
+      </c>
+      <c r="C474" t="n">
+        <v>3442</v>
+      </c>
+      <c r="D474" t="n">
+        <v>3447</v>
+      </c>
+      <c r="E474" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="475" ht="18.75" customHeight="1">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>تكملة على حسب المناسبة</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>{A18EDC94-F257-4FAC-99C7-0A8EA70F0FAF}</t>
+        </is>
+      </c>
+      <c r="C475" t="n">
+        <v>3448</v>
+      </c>
+      <c r="D475" t="n">
+        <v>3472</v>
+      </c>
+      <c r="E475" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="476" ht="18.75" customHeight="1">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>في حضور الاسقف</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>{A9183893-7B7E-459F-8547-F7A8F7D2D521}</t>
+        </is>
+      </c>
+      <c r="C476" t="n">
+        <v>3473</v>
+      </c>
+      <c r="D476" t="n">
+        <v>3481</v>
+      </c>
+      <c r="E476" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="477" ht="18.75" customHeight="1">
+      <c r="A477" t="inlineStr">
+        <is>
           <t>الختام 2</t>
         </is>
       </c>
-      <c r="B474" t="inlineStr">
+      <c r="B477" t="inlineStr">
         <is>
           <t>{A3DED752-5159-4F64-86F6-7B95F37A8327}</t>
         </is>
       </c>
-      <c r="C474" t="n">
-        <v>3474</v>
-      </c>
-      <c r="D474" t="n">
-        <v>3478</v>
-      </c>
-      <c r="E474" t="n">
+      <c r="C477" t="n">
+        <v>3482</v>
+      </c>
+      <c r="D477" t="n">
+        <v>3486</v>
+      </c>
+      <c r="E477" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10456,7 +10519,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10954,10 +11017,10 @@
         <v>825</v>
       </c>
       <c r="D23" t="n">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="E23" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" ht="18.75" customHeight="1">
@@ -10972,10 +11035,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="D24" t="n">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="E24" t="n">
         <v>17</v>
@@ -10993,10 +11056,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="D25" t="n">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="E25" t="n">
         <v>43</v>
@@ -11014,10 +11077,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="D26" t="n">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="E26" t="n">
         <v>11</v>
@@ -11035,10 +11098,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="D27" t="n">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="E27" t="n">
         <v>13</v>
@@ -11056,10 +11119,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="D28" t="n">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="E28" t="n">
         <v>16</v>
@@ -11077,10 +11140,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="D29" t="n">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="E29" t="n">
         <v>10</v>
@@ -11098,10 +11161,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D30" t="n">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="E30" t="n">
         <v>30</v>
@@ -11119,10 +11182,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="D31" t="n">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="E31" t="n">
         <v>51</v>
@@ -11140,10 +11203,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="D32" t="n">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="E32" t="n">
         <v>29</v>
@@ -11161,10 +11224,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="D33" t="n">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E33" t="n">
         <v>32</v>
@@ -11182,10 +11245,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="D34" t="n">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E34" t="n">
         <v>20</v>
@@ -11203,10 +11266,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="D35" t="n">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="E35" t="n">
         <v>57</v>
@@ -11224,10 +11287,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="D36" t="n">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="E36" t="n">
         <v>57</v>
@@ -11245,10 +11308,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="D37" t="n">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="E37" t="n">
         <v>61</v>
@@ -11266,10 +11329,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="D38" t="n">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="E38" t="n">
         <v>16</v>
@@ -11287,10 +11350,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="D39" t="n">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="E39" t="n">
         <v>17</v>
@@ -11308,10 +11371,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="D40" t="n">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="E40" t="n">
         <v>18</v>
@@ -11329,10 +11392,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="D41" t="n">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="E41" t="n">
         <v>30</v>
@@ -11350,10 +11413,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="D42" t="n">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="E42" t="n">
         <v>30</v>
@@ -11362,334 +11425,334 @@
     <row r="43" ht="18.75" customHeight="1">
       <c r="A43" t="inlineStr">
         <is>
-          <t>(سنوي) ابانا الذي في السموات</t>
+          <t>(التجلي) المجد لله ذي الرحمة</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>{55AD0713-7619-4F4A-BBF7-CBEC78E9D2B6}</t>
+          <t>{72B6A886-BE5B-444C-ADB8-80108ED1C462}</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="D43" t="n">
-        <v>1412</v>
+        <v>1414</v>
       </c>
       <c r="E43" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" ht="18.75" customHeight="1">
       <c r="A44" t="inlineStr">
         <is>
-          <t>(سنوي) اسمعوا يا شعب المسيح</t>
+          <t>(سنوي) ابانا الذي في السموات</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>{FBABEA1B-1917-427E-BD5E-EB2368CB6293}</t>
+          <t>{55AD0713-7619-4F4A-BBF7-CBEC78E9D2B6}</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1413</v>
+        <v>1415</v>
       </c>
       <c r="D44" t="n">
-        <v>1441</v>
+        <v>1428</v>
       </c>
       <c r="E44" t="n">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" ht="18.75" customHeight="1">
       <c r="A45" t="inlineStr">
         <is>
-          <t>(سنوي) المجد لمن رفع السموات</t>
+          <t>(سنوي) اسمعوا يا شعب المسيح</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>{12A69F25-ED75-4850-8C2A-4864364C2131}</t>
+          <t>{FBABEA1B-1917-427E-BD5E-EB2368CB6293}</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1442</v>
+        <v>1429</v>
       </c>
       <c r="D45" t="n">
-        <v>1472</v>
+        <v>1457</v>
       </c>
       <c r="E45" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" ht="18.75" customHeight="1">
       <c r="A46" t="inlineStr">
         <is>
-          <t>(سنوي) أول ما أبدي أسبح الإله</t>
+          <t>(سنوي) المجد لمن رفع السموات</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>{BA707332-FF09-40ED-BD05-0F3CE5931805}</t>
+          <t>{12A69F25-ED75-4850-8C2A-4864364C2131}</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1473</v>
+        <v>1458</v>
       </c>
       <c r="D46" t="n">
-        <v>1478</v>
+        <v>1488</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" ht="18.75" customHeight="1">
       <c r="A47" t="inlineStr">
         <is>
-          <t>الباب الثاني</t>
+          <t>(سنوي) أول ما أبدي أسبح الإله</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>{E9ED8CBA-74AF-4903-9BE7-83949A2E6042}</t>
+          <t>{BA707332-FF09-40ED-BD05-0F3CE5931805}</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1479</v>
+        <v>1489</v>
       </c>
       <c r="D47" t="n">
-        <v>1479</v>
+        <v>1518</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" ht="18.75" customHeight="1">
       <c r="A48" t="inlineStr">
         <is>
-          <t>أبادير وإيرائي اخته</t>
+          <t>الباب الثاني</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>{418E980F-1BC4-40C4-AED7-1DE2566AF0A8}</t>
+          <t>{E9ED8CBA-74AF-4903-9BE7-83949A2E6042}</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1480</v>
+        <v>1519</v>
       </c>
       <c r="D48" t="n">
-        <v>1504</v>
+        <v>1519</v>
       </c>
       <c r="E48" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" ht="18.75" customHeight="1">
       <c r="A49" t="inlineStr">
         <is>
-          <t>أبا اسخيرون القليني</t>
+          <t>أبادير وإيرائي اخته</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>{21D2DCA4-5857-4F13-886C-A79FCE9F45CF}</t>
+          <t>{418E980F-1BC4-40C4-AED7-1DE2566AF0A8}</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1505</v>
+        <v>1520</v>
       </c>
       <c r="D49" t="n">
-        <v>1516</v>
+        <v>1544</v>
       </c>
       <c r="E49" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" ht="18.75" customHeight="1">
       <c r="A50" t="inlineStr">
         <is>
-          <t>أباكراجون البتانوني</t>
+          <t>أبا اسخيرون القليني</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>{C6670786-A976-4B52-868E-171137C94BF0}</t>
+          <t>{21D2DCA4-5857-4F13-886C-A79FCE9F45CF}</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1517</v>
+        <v>1545</v>
       </c>
       <c r="D50" t="n">
-        <v>1532</v>
+        <v>1556</v>
       </c>
       <c r="E50" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" ht="18.75" customHeight="1">
       <c r="A51" t="inlineStr">
         <is>
-          <t>اباكير و يوحنا</t>
+          <t>أباكراجون البتانوني</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>{94B1CF6F-400F-4EBB-BEB3-7561B8B79E22}</t>
+          <t>{C6670786-A976-4B52-868E-171137C94BF0}</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1533</v>
+        <v>1557</v>
       </c>
       <c r="D51" t="n">
-        <v>1549</v>
+        <v>1572</v>
       </c>
       <c r="E51" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" ht="18.75" customHeight="1">
       <c r="A52" t="inlineStr">
         <is>
-          <t>أبانوب النهيسي</t>
+          <t>اباكير و يوحنا</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>{B7505EB8-9095-443D-8AB4-76B429FB6882}</t>
+          <t>{94B1CF6F-400F-4EBB-BEB3-7561B8B79E22}</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1550</v>
+        <v>1573</v>
       </c>
       <c r="D52" t="n">
-        <v>1565</v>
+        <v>1589</v>
       </c>
       <c r="E52" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" ht="18.75" customHeight="1">
       <c r="A53" t="inlineStr">
         <is>
-          <t>الأنبا إبرآم أسقف الفيوم</t>
+          <t>أبانوب النهيسي</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>{76A5C39E-E378-49E4-A1B3-3C3C6AD0FC45}</t>
+          <t>{B7505EB8-9095-443D-8AB4-76B429FB6882}</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1566</v>
+        <v>1590</v>
       </c>
       <c r="D53" t="n">
-        <v>1585</v>
+        <v>1605</v>
       </c>
       <c r="E53" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" ht="18.75" customHeight="1">
       <c r="A54" t="inlineStr">
         <is>
-          <t>الأنبا أبوللو والأنبا أبيب</t>
+          <t>الأنبا إبرآم أسقف الفيوم</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>{15F37CDF-162E-4235-B0CD-3EC560293C8F}</t>
+          <t>{76A5C39E-E378-49E4-A1B3-3C3C6AD0FC45}</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1586</v>
+        <v>1606</v>
       </c>
       <c r="D54" t="n">
-        <v>1604</v>
+        <v>1625</v>
       </c>
       <c r="E54" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" ht="18.75" customHeight="1">
       <c r="A55" t="inlineStr">
         <is>
-          <t>الشهيد مارجرجس الروماني</t>
+          <t>الأنبا أبوللو والأنبا أبيب</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>{FFF1B9FE-C89C-4F56-85B7-F375461AEA62}</t>
+          <t>{15F37CDF-162E-4235-B0CD-3EC560293C8F}</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1605</v>
+        <v>1626</v>
       </c>
       <c r="D55" t="n">
-        <v>1616</v>
+        <v>1644</v>
       </c>
       <c r="E55" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" ht="18.75" customHeight="1">
       <c r="A56" t="inlineStr">
         <is>
-          <t>القديس لوقا الانجيلي</t>
+          <t>الشهيد مارجرجس الروماني</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>{50EEB170-6F56-438C-943C-B8B3136DBB6A}</t>
+          <t>{FFF1B9FE-C89C-4F56-85B7-F375461AEA62}</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>1617</v>
+        <v>1645</v>
       </c>
       <c r="D56" t="n">
-        <v>1634</v>
+        <v>1656</v>
       </c>
       <c r="E56" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" ht="18.75" customHeight="1">
       <c r="A57" t="inlineStr">
         <is>
-          <t>القديس مارمرقس الرسول</t>
+          <t>القديس لوقا الانجيلي</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>{D4872368-E5CE-4B87-A314-70582CB26D33}</t>
+          <t>{50EEB170-6F56-438C-943C-B8B3136DBB6A}</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1635</v>
+        <v>1657</v>
       </c>
       <c r="D57" t="n">
-        <v>1653</v>
+        <v>1674</v>
       </c>
       <c r="E57" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" ht="18.75" customHeight="1">
       <c r="A58" t="inlineStr">
         <is>
-          <t>العذراء مريم</t>
+          <t>القديس مارمرقس الرسول</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>{BC31EDAD-70A8-41AD-8F09-30FB6E612B63}</t>
+          <t>{D4872368-E5CE-4B87-A314-70582CB26D33}</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1654</v>
+        <v>1675</v>
       </c>
       <c r="D58" t="n">
-        <v>1672</v>
+        <v>1693</v>
       </c>
       <c r="E58" t="n">
         <v>19</v>
@@ -11698,147 +11761,189 @@
     <row r="59" ht="18.75" customHeight="1">
       <c r="A59" t="inlineStr">
         <is>
-          <t>الملاك ميخائيل</t>
+          <t>العذراء مريم</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>{12793581-7FD0-4EE7-B903-2943F410A5D2}</t>
+          <t>{BC31EDAD-70A8-41AD-8F09-30FB6E612B63}</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1673</v>
+        <v>1694</v>
       </c>
       <c r="D59" t="n">
-        <v>1684</v>
+        <v>1712</v>
       </c>
       <c r="E59" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="60" ht="18.75" customHeight="1">
       <c r="A60" t="inlineStr">
         <is>
+          <t>الملاك ميخائيل</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>{12793581-7FD0-4EE7-B903-2943F410A5D2}</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>1713</v>
+      </c>
+      <c r="D60" t="n">
+        <v>1724</v>
+      </c>
+      <c r="E60" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" ht="18.75" customHeight="1">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>الملاك غبريال</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>{FFD2036A-0F2D-47E3-B5B9-AC167E3F6FF3}</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>1725</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1736</v>
+      </c>
+      <c r="E61" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" ht="18.75" customHeight="1">
+      <c r="A62" t="inlineStr">
+        <is>
           <t>الباب الثالث</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
+      <c r="B62" t="inlineStr">
         <is>
           <t>{E5B98BC1-9C9D-42EC-BB16-E848179FB9DC}</t>
         </is>
       </c>
-      <c r="C60" t="n">
-        <v>1685</v>
-      </c>
-      <c r="D60" t="n">
-        <v>1685</v>
-      </c>
-      <c r="E60" t="n">
+      <c r="C62" t="n">
+        <v>1737</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1737</v>
+      </c>
+      <c r="E62" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
+    <row r="63" ht="18.75" customHeight="1">
+      <c r="A63" t="inlineStr">
         <is>
           <t>رحلة الصوم الكبير</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
+      <c r="B63" t="inlineStr">
         <is>
           <t>{11755A37-6BDF-4E72-9537-F39867C5BB7D}</t>
         </is>
       </c>
-      <c r="C61" t="n">
-        <v>1686</v>
-      </c>
-      <c r="D61" t="n">
-        <v>1692</v>
-      </c>
-      <c r="E61" t="n">
+      <c r="C63" t="n">
+        <v>1738</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1744</v>
+      </c>
+      <c r="E63" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
+    <row r="64" ht="18.75" customHeight="1">
+      <c r="A64" t="inlineStr">
         <is>
           <t>عند شق الفجر باكر</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
+      <c r="B64" t="inlineStr">
         <is>
           <t>{D4859CD1-25CE-465C-846E-A0311D24DB66}</t>
         </is>
       </c>
-      <c r="C62" t="n">
-        <v>1693</v>
-      </c>
-      <c r="D62" t="n">
-        <v>1725</v>
-      </c>
-      <c r="E62" t="n">
+      <c r="C64" t="n">
+        <v>1745</v>
+      </c>
+      <c r="D64" t="n">
+        <v>1777</v>
+      </c>
+      <c r="E64" t="n">
         <v>33</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
+    <row r="65" ht="18.75" customHeight="1">
+      <c r="A65" t="inlineStr">
         <is>
           <t>قام حقا</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
+      <c r="B65" t="inlineStr">
         <is>
           <t>{4615B620-F94D-4CAD-843A-EB32E8369AAB}</t>
         </is>
       </c>
-      <c r="C63" t="n">
-        <v>1726</v>
-      </c>
-      <c r="D63" t="n">
-        <v>1739</v>
-      </c>
-      <c r="E63" t="n">
+      <c r="C65" t="n">
+        <v>1778</v>
+      </c>
+      <c r="D65" t="n">
+        <v>1791</v>
+      </c>
+      <c r="E65" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
+    <row r="66" ht="18.75" customHeight="1">
+      <c r="A66" t="inlineStr">
         <is>
           <t>انظروا يديه تأملوا رجليه</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr">
+      <c r="B66" t="inlineStr">
         <is>
           <t>{E1A31474-7F00-4B7D-90FD-A67415E32872}</t>
         </is>
       </c>
-      <c r="C64" t="n">
-        <v>1740</v>
-      </c>
-      <c r="D64" t="n">
-        <v>1754</v>
-      </c>
-      <c r="E64" t="n">
+      <c r="C66" t="n">
+        <v>1792</v>
+      </c>
+      <c r="D66" t="n">
+        <v>1806</v>
+      </c>
+      <c r="E66" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
+    <row r="67" ht="18.75" customHeight="1">
+      <c r="A67" t="inlineStr">
         <is>
           <t>يا ربنا مولى السلام</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
+      <c r="B67" t="inlineStr">
         <is>
           <t>{325B4DE6-FA63-4B6D-827F-BCC78EF1FEC9}</t>
         </is>
       </c>
-      <c r="C65" t="n">
-        <v>1755</v>
-      </c>
-      <c r="D65" t="n">
-        <v>1798</v>
-      </c>
-      <c r="E65" t="n">
+      <c r="C67" t="n">
+        <v>1807</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1850</v>
+      </c>
+      <c r="E67" t="n">
         <v>44</v>
       </c>
     </row>
@@ -24343,7 +24448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" ht="18.75" customHeight="1">
       <c r="A45" t="inlineStr">
         <is>
           <t>الشهيد فيلوباتير مرقوريوس</t>
@@ -24364,7 +24469,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" ht="18.75" customHeight="1">
       <c r="A46" t="inlineStr">
         <is>
           <t>الشهيد مارمينا</t>
@@ -24385,7 +24490,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" ht="18.75" customHeight="1">
       <c r="A47" t="inlineStr">
         <is>
           <t>الأنبا أنطونيوس</t>
@@ -24406,7 +24511,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" ht="18.75" customHeight="1">
       <c r="A48" t="inlineStr">
         <is>
           <t>الانبا بولا</t>
@@ -24427,7 +24532,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" ht="18.75" customHeight="1">
       <c r="A49" t="inlineStr">
         <is>
           <t>الأنبا بيشوى و الأنبا بولا</t>
@@ -24448,7 +24553,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" ht="18.75" customHeight="1">
       <c r="A50" t="inlineStr">
         <is>
           <t>ختام الذكصولوجيات</t>
@@ -24681,7 +24786,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26109,7 +26214,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" ht="18.75" customHeight="1">
       <c r="A68" t="inlineStr">
         <is>
           <t>ختام التسبحة</t>
@@ -26130,7 +26235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" ht="18.75" customHeight="1">
       <c r="A69" t="inlineStr">
         <is>
           <t>قدوس قدوس قدوس</t>
@@ -26145,10 +26250,31 @@
         <v>1611</v>
       </c>
       <c r="D69" t="n">
+        <v>1614</v>
+      </c>
+      <c r="E69" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>ابانا الذي في السموات</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>{68CD9B8E-B861-4695-8C6E-F8E0D19B6D78}</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
         <v>1615</v>
       </c>
-      <c r="E69" t="n">
-        <v>5</v>
+      <c r="D70" t="n">
+        <v>1615</v>
+      </c>
+      <c r="E70" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>